<commit_message>
Update Dot Plot Submission
</commit_message>
<xml_diff>
--- a/Dot Plot Submission.xlsx
+++ b/Dot Plot Submission.xlsx
@@ -47,13 +47,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
@@ -73,14 +72,11 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -124,8 +120,9 @@
     </c:title>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -135,37 +132,74 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:cat>
-            <c:strRef>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln cmpd="sng">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
               <c:f>Sheet1!$A$2:$A$9</c:f>
-            </c:strRef>
-          </c:cat>
-          <c:val>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Sheet1!$B$2:$B$9</c:f>
               <c:numCache/>
             </c:numRef>
-          </c:val>
+          </c:yVal>
         </c:ser>
-        <c:axId val="1832664093"/>
-        <c:axId val="1511715552"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="1832664093"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="821034531"/>
+        <c:axId val="1923054292"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="821034531"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -197,7 +231,10 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:spPr/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
@@ -212,10 +249,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1511715552"/>
-      </c:catAx>
+        <c:crossAx val="1923054292"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="1511715552"/>
+        <c:axId val="1923054292"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -290,7 +327,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1832664093"/>
+        <c:crossAx val="821034531"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -559,66 +596,66 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>22.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>20.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>25.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>20.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>35.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>15.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>15.0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>18.0</v>
       </c>
     </row>

</xml_diff>